<commit_message>
Added logout functionality to tests. Corrected some test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/AddEmployee.xlsx
+++ b/src/test/resources/AddEmployee.xlsx
@@ -91,13 +91,13 @@
     <t>Dev</t>
   </si>
   <si>
-    <t>Test.TestersonXIII</t>
-  </si>
-  <si>
-    <t>TestersonXIII</t>
-  </si>
-  <si>
-    <t>test.testersonxiii@orasi.com</t>
+    <t>Test.TestersonXIV</t>
+  </si>
+  <si>
+    <t>TestersonXIV</t>
+  </si>
+  <si>
+    <t>test.testersonxiv@orasi.com</t>
   </si>
 </sst>
 </file>
@@ -453,15 +453,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -471,7 +469,7 @@
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>

</xml_diff>